<commit_message>
Aqui vamos (antes del refactor de ResultadoQuinela)
</commit_message>
<xml_diff>
--- a/Documentos/Entidades.xlsx
+++ b/Documentos/Entidades.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13FF032-772C-4DAB-AE63-66A183745A4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2857DFBD-DAAC-457C-883D-14726B4A4242}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Liga</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>Crea una quinela para una jornada para un usuario</t>
+  </si>
+  <si>
+    <t>Jornadas/{jornadaId}</t>
+  </si>
+  <si>
+    <t>Devuelve la jornada con un Id determinado</t>
+  </si>
+  <si>
+    <t>Put</t>
+  </si>
+  <si>
+    <t>Abre/cierra la jornada al publico para que se creen quinelas</t>
   </si>
 </sst>
 </file>
@@ -412,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF18"/>
+  <dimension ref="A1:AF20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B13:B14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,80 +508,102 @@
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
+      <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>